<commit_message>
update handling of products
</commit_message>
<xml_diff>
--- a/data/input-data/data-definitions.xlsx
+++ b/data/input-data/data-definitions.xlsx
@@ -4,12 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22624"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="14980" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="HiddenValidation" sheetId="16" state="hidden" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="20" r:id="rId2"/>
     <sheet name="Reference Data" sheetId="18" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="21" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="22" r:id="rId5"/>
+    <sheet name="Sheet4" sheetId="23" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_HidValB1B46">HiddenValidation!$B$1:$B$46</definedName>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="374">
   <si>
     <t>BIGINT</t>
   </si>
@@ -278,9 +281,6 @@
     <t>IC Tomorrow</t>
   </si>
   <si>
-    <t>Centre of Excellence</t>
-  </si>
-  <si>
     <t>Special Interest Group</t>
   </si>
   <si>
@@ -332,9 +332,6 @@
     <t>IV</t>
   </si>
   <si>
-    <t>Large</t>
-  </si>
-  <si>
     <t>SBRI</t>
   </si>
   <si>
@@ -344,18 +341,6 @@
     <t>EPES</t>
   </si>
   <si>
-    <t>ADVM</t>
-  </si>
-  <si>
-    <t>DEVL</t>
-  </si>
-  <si>
-    <t>I_CT</t>
-  </si>
-  <si>
-    <t>HIVM</t>
-  </si>
-  <si>
     <t>HLTHCR</t>
   </si>
   <si>
@@ -374,9 +359,6 @@
     <t>TECH</t>
   </si>
   <si>
-    <t>SUST</t>
-  </si>
-  <si>
     <t>DIGS</t>
   </si>
   <si>
@@ -452,9 +434,6 @@
     <t>Enabling technology capability</t>
   </si>
   <si>
-    <t>BIO</t>
-  </si>
-  <si>
     <t>SPCC</t>
   </si>
   <si>
@@ -521,9 +500,6 @@
     <t>Integrated Transport</t>
   </si>
   <si>
-    <t>DIIA</t>
-  </si>
-  <si>
     <t>Stratified Medicine</t>
   </si>
   <si>
@@ -626,12 +602,6 @@
     <t>A type of Product that provides a process to identify the best Applicants to take part in a Project  or receive Funding for a specific innovation</t>
   </si>
   <si>
-    <t>A type of Internal Organisation accountable and responsible for the delivery of the TSB objectives within an identified Area</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A defined  segment of UK technology  knowledge and experience identified in the TSB Strategy and Delivery Plan for investment with a defined budgeted commitment. Also used as a division of  Internal Organisation </t>
-  </si>
-  <si>
     <t>An enabling technology in key sectors including construction, clean tech and transport</t>
   </si>
   <si>
@@ -764,9 +734,6 @@
     <t>A  type of Competition for Funding designed for short term, business led collaborative projects</t>
   </si>
   <si>
-    <t>Establishment of specialist facilities and capability to provide a hub for innovation in specific technology area</t>
-  </si>
-  <si>
     <t>Resource Efficiency</t>
   </si>
   <si>
@@ -776,37 +743,19 @@
     <t>HVS</t>
   </si>
   <si>
-    <t>ASSL</t>
-  </si>
-  <si>
     <t>STMD</t>
   </si>
   <si>
-    <t>LIBG</t>
-  </si>
-  <si>
     <t>RSEF</t>
   </si>
   <si>
-    <t>SAF</t>
-  </si>
-  <si>
-    <t>WTEX</t>
-  </si>
-  <si>
     <t>AERO</t>
   </si>
   <si>
-    <t>LCV</t>
-  </si>
-  <si>
     <t>ITRAN</t>
   </si>
   <si>
     <t>Detection and Identification of Infectious Agents</t>
-  </si>
-  <si>
-    <t>All Thematic Area</t>
   </si>
   <si>
     <t>All TSB Programmes</t>
@@ -879,9 +828,6 @@
     <t>Innovative developments using satellite data and space-based satellite systems</t>
   </si>
   <si>
-    <t>A TSB high level category for Thematic Area</t>
-  </si>
-  <si>
     <t>Accelerating the early pre-commercial stages of technology demonstration and commercialisation</t>
   </si>
   <si>
@@ -924,17 +870,293 @@
     <t>Implementing a Creative Industries Technology Strategy with emphasis on meta-data, cross platform interoperability and prompting knowledge exchange</t>
   </si>
   <si>
-    <t>TSB Programme  / Budget Area</t>
-  </si>
-  <si>
-    <t>Priority Area</t>
+    <t>ADV_MAT</t>
+  </si>
+  <si>
+    <t>AGRI_FD</t>
+  </si>
+  <si>
+    <t>ASS_LIV</t>
+  </si>
+  <si>
+    <t>BIO_SCI</t>
+  </si>
+  <si>
+    <t>CRE_IND</t>
+  </si>
+  <si>
+    <t>DET_IIA</t>
+  </si>
+  <si>
+    <t>E_P_E_S</t>
+  </si>
+  <si>
+    <t>ENV_SUS</t>
+  </si>
+  <si>
+    <t>HIVAMAN</t>
+  </si>
+  <si>
+    <t>INFO_CT</t>
+  </si>
+  <si>
+    <t>ITS_SER</t>
+  </si>
+  <si>
+    <t>LEG_CRD</t>
+  </si>
+  <si>
+    <t>LEG_ENE</t>
+  </si>
+  <si>
+    <t>LOC_VEH</t>
+  </si>
+  <si>
+    <t>LOW_IMP</t>
+  </si>
+  <si>
+    <t>LP_ENRG</t>
+  </si>
+  <si>
+    <t>LP_ENVT</t>
+  </si>
+  <si>
+    <t>LP_HIVA</t>
+  </si>
+  <si>
+    <t>LP_INFO</t>
+  </si>
+  <si>
+    <t>NANOTEC</t>
+  </si>
+  <si>
+    <t>NET_SEC</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>TRANSPO</t>
+  </si>
+  <si>
+    <t>HVM</t>
+  </si>
+  <si>
+    <t>ADVMAT</t>
+  </si>
+  <si>
+    <t>BIOS</t>
+  </si>
+  <si>
+    <t>IBIOT</t>
+  </si>
+  <si>
+    <t>Establishment of specialist facilities and capability to provide a hub for innovation in specific technology area as a centre of excellence</t>
+  </si>
+  <si>
+    <t>Centre</t>
+  </si>
+  <si>
+    <t>Theme</t>
+  </si>
+  <si>
+    <t>A division of  Internal Organisation for Budget control aligned to the Theme</t>
+  </si>
+  <si>
+    <t>A TSB high level category for Theme</t>
+  </si>
+  <si>
+    <t>All Themes</t>
+  </si>
+  <si>
+    <t>An individual or group accountable and responsible for the delivery of the TSB objectives within a part of an identified  Area</t>
+  </si>
+  <si>
+    <t>A defined  segment of UK technology  knowledge and experience identified in the TSB Strategy and Delivery Plan for investment with a defined budgeted commitment.  Synonym Thematic  or Priority Area</t>
+  </si>
+  <si>
+    <t>Legacy Energy</t>
+  </si>
+  <si>
+    <t>Large Project Environment</t>
+  </si>
+  <si>
+    <t>Large Project High Value Manufacturing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Large Project Information &amp; Communication Technology </t>
+  </si>
+  <si>
+    <t>Nanotechnology</t>
+  </si>
+  <si>
+    <t>Network Security</t>
+  </si>
+  <si>
+    <t>Teams from Reference Data</t>
+  </si>
+  <si>
+    <t>Teams from FOI</t>
+  </si>
+  <si>
+    <t>Catapults</t>
+  </si>
+  <si>
+    <t>Detection &amp; Identification of Infectious Agents</t>
+  </si>
+  <si>
+    <t>Digital Britain</t>
+  </si>
+  <si>
+    <t>Electronics, Photonics &amp; Electrical Systems</t>
+  </si>
+  <si>
+    <t>Energy Generation &amp; Supply</t>
+  </si>
+  <si>
+    <t>Energy Technology</t>
+  </si>
+  <si>
+    <t>Environmental Sustainability</t>
+  </si>
+  <si>
+    <t>European: Information &amp; Communication Technology</t>
+  </si>
+  <si>
+    <t>European: Small Business Research Inititiative</t>
+  </si>
+  <si>
+    <t>Except.- Low Carbon Vechicles</t>
+  </si>
+  <si>
+    <t>Grant for R&amp;D</t>
+  </si>
+  <si>
+    <t>Information &amp; Communication Technology</t>
+  </si>
+  <si>
+    <t>Innovation Platform</t>
+  </si>
+  <si>
+    <t>Intelligent Transport Systems</t>
+  </si>
+  <si>
+    <t>Knowledge Transfer Partnerships</t>
+  </si>
+  <si>
+    <t>Large Projects: Energy</t>
+  </si>
+  <si>
+    <t>Large Projects: Environment</t>
+  </si>
+  <si>
+    <t>Large Projects: High Value Manufacturing</t>
+  </si>
+  <si>
+    <t>Large Projects: Information &amp; Communications Technology</t>
+  </si>
+  <si>
+    <t>Large Projects: Transport</t>
+  </si>
+  <si>
+    <t>Legacy  RDA Grant for R&amp;D</t>
+  </si>
+  <si>
+    <t>Legacy: Collaborative Research &amp; Development</t>
+  </si>
+  <si>
+    <t>Legacy: Energy</t>
+  </si>
+  <si>
+    <t>Legacy: Regional Development Agency Grant for Research &amp; Development</t>
+  </si>
+  <si>
+    <t>Medicines &amp; Healthcare</t>
+  </si>
+  <si>
+    <t>Responsive</t>
+  </si>
+  <si>
+    <t>Space Programmes</t>
+  </si>
+  <si>
+    <t>Sustainable Agri-Food Protection</t>
+  </si>
+  <si>
+    <t>Transport: Aerospace</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>LCHPD</t>
+  </si>
+  <si>
+    <t>Funding for a large scale demonstrator  in Environment Area</t>
+  </si>
+  <si>
+    <t>Funding for a large scale demonstrator  in High Value Manufacturing Area</t>
+  </si>
+  <si>
+    <t>Funding for a large scale demonstrator  in Information &amp; Communication TEchnologyArea</t>
+  </si>
+  <si>
+    <t>Large Project Energy</t>
+  </si>
+  <si>
+    <t>Funding for a large scale demonstrator  in Energy Area</t>
+  </si>
+  <si>
+    <t>Intelligent Transport Services</t>
+  </si>
+  <si>
+    <t>AreaName (Dedupe from FOI)</t>
+  </si>
+  <si>
+    <t>TSB Programmes</t>
+  </si>
+  <si>
+    <t>Funding for a large scale demonstrator in Transport Area</t>
+  </si>
+  <si>
+    <t>Funding previously provided for  projects in the Energy Area prior to establishment of Technology Strategy Board</t>
+  </si>
+  <si>
+    <t>Funding previously provided for Collaborative Research and Development prior to establishment of Technology Strategy Board</t>
+  </si>
+  <si>
+    <t>Funding previously provided by Regional Developemnet Agencies for Research and Development prior to establishment of Technology Strategy Board</t>
+  </si>
+  <si>
+    <t>Funding for projects in the Energy Area specifically aimed at its sourcing and distribution</t>
+  </si>
+  <si>
+    <t>Funding assigned from European sources managed by Technology Strategy Board for projects in the Information and Communication Technology Area</t>
+  </si>
+  <si>
+    <t>Funding assigned from European sources managed by Technology Strategy Board for Small Businesss research</t>
+  </si>
+  <si>
+    <t>A type of competition run regularly for ideas in any technology area including thematic ones</t>
+  </si>
+  <si>
+    <t>Application of technology at  atomic and molecular levels to materials</t>
+  </si>
+  <si>
+    <t>Ensuring the challenges of security are addressed within the Digital Economy</t>
+  </si>
+  <si>
+    <t>A grant scheme (now termed SMART) which offers funding to small  and medium-sized enterprises (SMEs) to engage in R&amp;D projects in the strategically important areas of science, engineering and technology, from which successful new products, processes and services could emerge.</t>
+  </si>
+  <si>
+    <t>A specific  area for reducing carbon and other environmentally harmful emissions from all vehicles and increasing their efficiency</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -971,11 +1193,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="14"/>
       <color theme="1"/>
@@ -1003,8 +1220,25 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="72"/>
+      <name val="SansSerif"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="SansSerif"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1032,6 +1266,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="31"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1082,7 +1334,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1093,10 +1345,10 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1111,7 +1363,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1156,7 +1408,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1165,7 +1417,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1177,7 +1429,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1185,8 +1437,46 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1799,10 +2089,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B5"/>
+  <dimension ref="A2:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1816,7 +2106,7 @@
         <v>49</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="28">
@@ -1824,23 +2114,31 @@
         <v>46</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="43">
       <c r="A4" s="32" t="s">
-        <v>197</v>
+        <v>309</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="28">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15">
       <c r="A5" s="32" t="s">
+        <v>188</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="28">
+      <c r="A6" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>200</v>
+      <c r="B6" s="1" t="s">
+        <v>313</v>
       </c>
     </row>
   </sheetData>
@@ -1856,41 +2154,41 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F91"/>
+  <dimension ref="A1:G111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="D103" sqref="D103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="31.1640625" style="21" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" style="21"/>
+    <col min="1" max="1" width="8.5" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="21" customWidth="1"/>
     <col min="3" max="3" width="45.1640625" style="22" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="92.5" style="23" customWidth="1"/>
     <col min="5" max="5" width="29" style="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="52.6640625" style="21" customWidth="1"/>
+    <col min="6" max="6" width="33.5" style="21" customWidth="1"/>
     <col min="7" max="16384" width="8.83203125" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1" ht="18">
       <c r="A1" s="4" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>54</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="10" customFormat="1" ht="28">
@@ -1898,33 +2196,33 @@
         <v>49</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>46</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="10" customFormat="1" ht="18">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="10" customFormat="1" ht="28">
       <c r="A3" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>84</v>
+        <v>308</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>246</v>
+        <v>307</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="10" customFormat="1" ht="18">
@@ -1932,16 +2230,16 @@
         <v>49</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>48</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="10" customFormat="1" ht="18">
@@ -1949,16 +2247,16 @@
         <v>49</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="10" customFormat="1" ht="18">
@@ -1966,13 +2264,13 @@
         <v>49</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>46</v>
@@ -1983,13 +2281,13 @@
         <v>49</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>46</v>
@@ -2000,13 +2298,13 @@
         <v>49</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>55</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>46</v>
@@ -2017,19 +2315,19 @@
         <v>49</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>78</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="F9" s="31" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="6" customFormat="1">
@@ -2037,187 +2335,172 @@
         <v>49</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>46</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="6" customFormat="1">
-      <c r="A11" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>245</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" s="6" customFormat="1" ht="28">
+      <c r="B11" s="12"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="1:6" s="6" customFormat="1">
       <c r="A12" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>217</v>
+        <v>234</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" s="6" customFormat="1">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="6" customFormat="1" ht="28">
       <c r="A13" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>83</v>
+        <v>59</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>232</v>
+        <v>206</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F13" s="34" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" s="6" customFormat="1" ht="28">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="6" customFormat="1">
       <c r="A14" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="F14" s="31" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" s="6" customFormat="1" ht="56">
+        <v>46</v>
+      </c>
+      <c r="F14" s="34" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="6" customFormat="1" ht="28">
       <c r="A15" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>171</v>
+        <v>81</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>205</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" s="6" customFormat="1">
+        <v>165</v>
+      </c>
+      <c r="F15" s="31" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="6" customFormat="1" ht="84">
       <c r="A16" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>234</v>
+        <v>51</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>162</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" s="6" customFormat="1" ht="42">
+        <v>165</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="6" customFormat="1">
       <c r="A17" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>53</v>
+        <v>86</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F17" s="35" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" s="6" customFormat="1">
+    </row>
+    <row r="18" spans="1:6" s="6" customFormat="1" ht="56">
       <c r="A18" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>179</v>
+        <v>353</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>89</v>
+        <v>53</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>170</v>
+        <v>229</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" s="6" customFormat="1" ht="28">
+      <c r="F18" s="35" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="6" customFormat="1">
       <c r="A19" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>103</v>
+        <v>170</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>230</v>
+        <v>161</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="F19" s="35" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="6" customFormat="1" ht="42">
@@ -2225,50 +2508,53 @@
         <v>49</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>177</v>
+        <v>101</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="D20" s="33" t="s">
-        <v>224</v>
+        <v>80</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>219</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" s="6" customFormat="1">
+        <v>46</v>
+      </c>
+      <c r="F20" s="35" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="6" customFormat="1" ht="42">
       <c r="A21" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>123</v>
+        <v>168</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>226</v>
+        <v>57</v>
+      </c>
+      <c r="D21" s="33" t="s">
+        <v>213</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" s="6" customFormat="1" ht="28">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="6" customFormat="1">
       <c r="A22" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>236</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>48</v>
+        <v>215</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="6" customFormat="1" ht="28">
@@ -2276,34 +2562,36 @@
         <v>49</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>94</v>
+        <v>120</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>96</v>
+        <v>56</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>225</v>
       </c>
       <c r="E23" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="F23" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" s="6" customFormat="1">
+    </row>
+    <row r="24" spans="1:6" s="6" customFormat="1" ht="28">
       <c r="A24" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>122</v>
+        <v>93</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="D24" s="9"/>
+        <v>77</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>95</v>
+      </c>
       <c r="E24" s="11" t="s">
         <v>48</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="6" customFormat="1">
@@ -2311,58 +2599,53 @@
         <v>49</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>237</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="D25" s="9"/>
       <c r="E25" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" s="6" customFormat="1" ht="28">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="6" customFormat="1">
       <c r="A26" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>82</v>
+        <v>119</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>242</v>
+        <v>226</v>
       </c>
       <c r="E26" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="F26" s="34" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" s="6" customFormat="1">
+      <c r="F26" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="6" customFormat="1" ht="28">
       <c r="A27" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>130</v>
+        <v>82</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="E27" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="F27" s="34" t="s">
         <v>228</v>
       </c>
     </row>
@@ -2371,16 +2654,19 @@
         <v>49</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>152</v>
+        <v>123</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>145</v>
+        <v>56</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="6" customFormat="1">
@@ -2388,16 +2674,16 @@
         <v>49</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="6" customFormat="1">
@@ -2405,16 +2691,16 @@
         <v>49</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>225</v>
+        <v>208</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>87</v>
+        <v>137</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="6" customFormat="1">
@@ -2422,1037 +2708,1358 @@
         <v>49</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>180</v>
+        <v>141</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>183</v>
+        <v>142</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" s="6" customFormat="1" ht="28">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" s="6" customFormat="1">
       <c r="A32" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="E32" s="11" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="6" customFormat="1">
+    <row r="33" spans="1:7" s="6" customFormat="1" ht="28">
       <c r="A33" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="E33" s="11" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="6" customFormat="1">
-      <c r="B34" s="12"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="11"/>
-    </row>
-    <row r="35" spans="1:6" s="14" customFormat="1">
-      <c r="A35" s="14" t="s">
-        <v>300</v>
-      </c>
-      <c r="B35" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="C35" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="D35" s="16" t="s">
-        <v>284</v>
-      </c>
-      <c r="E35" s="18" t="s">
-        <v>260</v>
-      </c>
-      <c r="F35" s="14" t="s">
+    <row r="34" spans="1:7" s="6" customFormat="1">
+      <c r="A34" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" s="12" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" s="14" customFormat="1">
+      <c r="C34" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" s="6" customFormat="1">
+      <c r="B35" s="12"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="11"/>
+    </row>
+    <row r="36" spans="1:7" s="14" customFormat="1">
       <c r="A36" s="14" t="s">
-        <v>300</v>
+        <v>309</v>
       </c>
       <c r="B36" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>311</v>
+      </c>
+      <c r="E36" s="18" t="s">
+        <v>312</v>
+      </c>
+      <c r="F36" s="14" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" s="14" customFormat="1">
+      <c r="A37" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="C37" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="C36" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="D36" s="16" t="s">
-        <v>284</v>
-      </c>
-      <c r="E36" s="18" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" s="14" customFormat="1">
-      <c r="A37" s="14" t="s">
-        <v>300</v>
-      </c>
-      <c r="B37" s="15" t="s">
+      <c r="D37" s="16" t="s">
+        <v>311</v>
+      </c>
+      <c r="E37" s="18" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" s="14" customFormat="1">
+      <c r="A38" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>311</v>
+      </c>
+      <c r="E38" s="18" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" s="14" customFormat="1">
+      <c r="A39" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="B39" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>311</v>
+      </c>
+      <c r="E39" s="18" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" s="14" customFormat="1">
+      <c r="A40" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="B40" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="C37" s="16" t="s">
+      <c r="C40" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>311</v>
+      </c>
+      <c r="E40" s="18" t="s">
+        <v>312</v>
+      </c>
+      <c r="G40" s="36"/>
+    </row>
+    <row r="41" spans="1:7" s="14" customFormat="1">
+      <c r="A41" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="B41" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="E41" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="G41" s="41" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" s="14" customFormat="1">
+      <c r="A42" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>305</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D42" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="E42" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="G42" s="36" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" s="14" customFormat="1">
+      <c r="A43" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D43" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="E43" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="G43" s="39"/>
+    </row>
+    <row r="44" spans="1:7" s="14" customFormat="1">
+      <c r="A44" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="B44" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="C44" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D44" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="E44" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="D37" s="16" t="s">
-        <v>284</v>
-      </c>
-      <c r="E37" s="18" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" s="14" customFormat="1">
-      <c r="A38" s="14" t="s">
-        <v>300</v>
-      </c>
-      <c r="B38" s="19" t="s">
-        <v>134</v>
-      </c>
-      <c r="C38" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="D38" s="16" t="s">
-        <v>284</v>
-      </c>
-      <c r="E38" s="18" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" s="14" customFormat="1">
-      <c r="A39" s="14" t="s">
-        <v>300</v>
-      </c>
-      <c r="B39" s="19" t="s">
-        <v>143</v>
-      </c>
-      <c r="C39" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="D39" s="16" t="s">
-        <v>284</v>
-      </c>
-      <c r="E39" s="18" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" s="14" customFormat="1">
-      <c r="A40" s="14" t="s">
-        <v>300</v>
-      </c>
-      <c r="B40" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="C40" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="D40" s="17" t="s">
-        <v>204</v>
-      </c>
-      <c r="E40" s="14" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" s="14" customFormat="1">
-      <c r="A41" s="14" t="s">
-        <v>300</v>
-      </c>
-      <c r="B41" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="C41" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="D41" s="17" t="s">
-        <v>207</v>
-      </c>
-      <c r="E41" s="14" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" s="14" customFormat="1">
-      <c r="A42" s="14" t="s">
-        <v>300</v>
-      </c>
-      <c r="B42" s="19" t="s">
+      <c r="G44" s="37"/>
+    </row>
+    <row r="45" spans="1:7" s="14" customFormat="1">
+      <c r="A45" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="B45" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="C45" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="D45" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="E45" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" s="14" customFormat="1">
+      <c r="A46" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="B46" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="C42" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="D42" s="17" t="s">
-        <v>208</v>
-      </c>
-      <c r="E42" s="14" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" s="14" customFormat="1">
-      <c r="A43" s="14" t="s">
-        <v>300</v>
-      </c>
-      <c r="B43" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="C43" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="D43" s="17" t="s">
-        <v>211</v>
-      </c>
-      <c r="E43" s="14" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" s="14" customFormat="1">
-      <c r="A44" s="14" t="s">
-        <v>300</v>
-      </c>
-      <c r="B44" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="C44" s="16" t="s">
+      <c r="C46" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="D44" s="17" t="s">
-        <v>205</v>
-      </c>
-      <c r="E44" s="14" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" s="14" customFormat="1">
-      <c r="A45" s="14" t="s">
-        <v>300</v>
-      </c>
-      <c r="B45" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="C45" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="D45" s="17" t="s">
-        <v>209</v>
-      </c>
-      <c r="E45" s="14" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" s="14" customFormat="1">
-      <c r="A46" s="14" t="s">
-        <v>300</v>
-      </c>
-      <c r="B46" s="20" t="s">
-        <v>191</v>
-      </c>
-      <c r="C46" s="16" t="s">
-        <v>73</v>
-      </c>
       <c r="D46" s="17" t="s">
-        <v>215</v>
+        <v>194</v>
       </c>
       <c r="E46" s="14" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" s="14" customFormat="1">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" s="14" customFormat="1">
       <c r="A47" s="14" t="s">
-        <v>300</v>
-      </c>
-      <c r="B47" s="20" t="s">
-        <v>190</v>
+        <v>309</v>
+      </c>
+      <c r="B47" s="19" t="s">
+        <v>103</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="D47" s="17" t="s">
-        <v>213</v>
+        <v>195</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" s="14" customFormat="1">
+        <v>132</v>
+      </c>
+      <c r="G47" s="36" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" s="14" customFormat="1">
       <c r="A48" s="14" t="s">
-        <v>300</v>
+        <v>309</v>
       </c>
       <c r="B48" s="20" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="C48" s="16" t="s">
         <v>75</v>
       </c>
       <c r="D48" s="17" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="E48" s="14" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="49" spans="1:6" s="14" customFormat="1">
+    <row r="49" spans="1:7" s="14" customFormat="1">
       <c r="A49" s="14" t="s">
-        <v>300</v>
+        <v>309</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>178</v>
+        <v>105</v>
       </c>
       <c r="C49" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D49" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="E49" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="G49" s="41"/>
+    </row>
+    <row r="50" spans="1:7" s="14" customFormat="1">
+      <c r="A50" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="B50" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="C50" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="D49" s="17" t="s">
-        <v>212</v>
-      </c>
-      <c r="E49" s="14" t="s">
+      <c r="D50" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="E50" s="14" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" s="14" customFormat="1">
-      <c r="A50" s="14" t="s">
-        <v>300</v>
-      </c>
-      <c r="B50" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="C50" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="D50" s="17" t="s">
-        <v>202</v>
-      </c>
-      <c r="E50" s="14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" s="14" customFormat="1">
+      <c r="G50" s="36" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" s="14" customFormat="1">
       <c r="A51" s="14" t="s">
-        <v>300</v>
+        <v>309</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>142</v>
+        <v>104</v>
       </c>
       <c r="C51" s="16" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D51" s="17" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="E51" s="14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" s="14" customFormat="1">
+        <v>130</v>
+      </c>
+      <c r="G51" s="36"/>
+    </row>
+    <row r="52" spans="1:7" s="14" customFormat="1">
       <c r="A52" s="14" t="s">
-        <v>300</v>
+        <v>309</v>
       </c>
       <c r="B52" s="19" t="s">
-        <v>105</v>
+        <v>303</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="D52" s="17" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="E52" s="14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" s="14" customFormat="1">
+        <v>131</v>
+      </c>
+      <c r="G52" s="39"/>
+    </row>
+    <row r="53" spans="1:7" s="14" customFormat="1">
       <c r="A53" s="14" t="s">
-        <v>300</v>
+        <v>309</v>
       </c>
       <c r="B53" s="19" t="s">
-        <v>108</v>
+        <v>67</v>
       </c>
       <c r="C53" s="16" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="D53" s="17" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="E53" s="14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" s="14" customFormat="1">
+        <v>132</v>
+      </c>
+      <c r="G53" s="37" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" s="14" customFormat="1">
       <c r="A54" s="14" t="s">
-        <v>300</v>
+        <v>309</v>
       </c>
       <c r="B54" s="19" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="C54" s="16" t="s">
         <v>72</v>
       </c>
       <c r="D54" s="16" t="s">
+        <v>265</v>
+      </c>
+      <c r="E54" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="G54" s="37" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" s="14" customFormat="1">
+      <c r="A55" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="B55" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="C55" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="D55" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="E55" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="G55" s="36"/>
+    </row>
+    <row r="56" spans="1:7" s="14" customFormat="1">
+      <c r="B56" s="19"/>
+      <c r="C56" s="16"/>
+      <c r="D56" s="17"/>
+      <c r="G56" s="37" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" s="27" customFormat="1">
+      <c r="A57" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B57" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="C57" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="D57" s="26" t="s">
+        <v>252</v>
+      </c>
+      <c r="E57" s="24" t="s">
+        <v>243</v>
+      </c>
+      <c r="F57" s="27" t="s">
+        <v>253</v>
+      </c>
+      <c r="G57" s="36" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" s="27" customFormat="1" ht="28">
+      <c r="A58" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B58" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="C58" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="D58" s="26" t="s">
+        <v>248</v>
+      </c>
+      <c r="E58" s="24" t="s">
+        <v>243</v>
+      </c>
+      <c r="F58" s="27" t="s">
+        <v>253</v>
+      </c>
+      <c r="G58" s="36" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" s="27" customFormat="1" ht="42">
+      <c r="A59" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B59" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="C59" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="D59" s="26" t="s">
+        <v>244</v>
+      </c>
+      <c r="E59" s="24" t="s">
+        <v>243</v>
+      </c>
+      <c r="F59" s="27" t="s">
+        <v>253</v>
+      </c>
+      <c r="G59" s="37" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" s="27" customFormat="1" ht="28">
+      <c r="A60" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B60" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="C60" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D60" s="26" t="s">
+        <v>245</v>
+      </c>
+      <c r="E60" s="24" t="s">
+        <v>243</v>
+      </c>
+      <c r="F60" s="27" t="s">
+        <v>253</v>
+      </c>
+      <c r="G60" s="36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" s="27" customFormat="1" ht="28">
+      <c r="A61" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B61" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="C61" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="D61" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="E61" s="24" t="s">
+        <v>243</v>
+      </c>
+      <c r="F61" s="27" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" s="27" customFormat="1" ht="28">
+      <c r="A62" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B62" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="C62" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="D62" s="26" t="s">
+        <v>247</v>
+      </c>
+      <c r="E62" s="24" t="s">
+        <v>243</v>
+      </c>
+      <c r="F62" s="27" t="s">
+        <v>253</v>
+      </c>
+      <c r="G62" s="36"/>
+    </row>
+    <row r="63" spans="1:7" s="27" customFormat="1">
+      <c r="A63" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B63" s="36" t="s">
+        <v>287</v>
+      </c>
+      <c r="C63" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="D63" s="26" t="s">
+        <v>250</v>
+      </c>
+      <c r="E63" s="24" t="s">
+        <v>243</v>
+      </c>
+      <c r="F63" s="27" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" s="27" customFormat="1" ht="17.25" customHeight="1">
+      <c r="A64" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B64" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="C64" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D64" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="E64" s="24" t="s">
+        <v>243</v>
+      </c>
+      <c r="F64" s="27" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" s="27" customFormat="1" ht="42">
+      <c r="A65" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B65" s="36" t="s">
+        <v>302</v>
+      </c>
+      <c r="C65" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="D65" s="26" t="s">
+        <v>249</v>
+      </c>
+      <c r="E65" s="24" t="s">
+        <v>243</v>
+      </c>
+      <c r="F65" s="27" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" s="27" customFormat="1" ht="28">
+      <c r="A66" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B66" s="40" t="s">
+        <v>280</v>
+      </c>
+      <c r="C66" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="D66" s="26" t="s">
+        <v>274</v>
+      </c>
+      <c r="E66" s="24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" s="27" customFormat="1" ht="28">
+      <c r="A67" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B67" s="25" t="s">
+        <v>240</v>
+      </c>
+      <c r="C67" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D67" s="26" t="s">
+        <v>277</v>
+      </c>
+      <c r="E67" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" s="27" customFormat="1">
+      <c r="A68" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B68" s="40" t="s">
+        <v>282</v>
+      </c>
+      <c r="C68" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="D68" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="E68" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" s="27" customFormat="1" ht="28">
+      <c r="A69" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B69" s="36" t="s">
         <v>283</v>
       </c>
-      <c r="E54" s="14" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" s="14" customFormat="1">
-      <c r="B55" s="19"/>
-      <c r="C55" s="16"/>
-      <c r="D55" s="17"/>
-    </row>
-    <row r="56" spans="1:6" s="27" customFormat="1">
-      <c r="A56" s="24" t="s">
-        <v>299</v>
-      </c>
-      <c r="B56" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="C56" s="24" t="s">
+      <c r="C69" s="28" t="s">
+        <v>272</v>
+      </c>
+      <c r="D69" s="26" t="s">
+        <v>273</v>
+      </c>
+      <c r="E69" s="24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" s="27" customFormat="1" ht="28">
+      <c r="A70" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B70" s="40" t="s">
+        <v>284</v>
+      </c>
+      <c r="C70" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="D70" s="26" t="s">
+        <v>279</v>
+      </c>
+      <c r="E70" s="24" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" s="27" customFormat="1" ht="28">
+      <c r="A71" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B71" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="C71" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="D71" s="26" t="s">
+        <v>258</v>
+      </c>
+      <c r="E71" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="D56" s="26" t="s">
-        <v>270</v>
-      </c>
-      <c r="E56" s="24" t="s">
-        <v>261</v>
-      </c>
-      <c r="F56" s="27" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" s="27" customFormat="1" ht="28">
-      <c r="A57" s="24" t="s">
-        <v>299</v>
-      </c>
-      <c r="B57" s="25" t="s">
-        <v>117</v>
-      </c>
-      <c r="C57" s="24" t="s">
-        <v>167</v>
-      </c>
-      <c r="D57" s="26" t="s">
+    </row>
+    <row r="72" spans="1:6" s="27" customFormat="1" ht="28">
+      <c r="A72" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B72" s="40" t="s">
+        <v>285</v>
+      </c>
+      <c r="C72" s="24" t="s">
+        <v>242</v>
+      </c>
+      <c r="D72" s="26" t="s">
+        <v>262</v>
+      </c>
+      <c r="E72" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" s="27" customFormat="1" ht="28">
+      <c r="A73" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B73" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="C73" s="24" t="s">
+        <v>185</v>
+      </c>
+      <c r="D73" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="E73" s="24" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" s="27" customFormat="1">
+      <c r="A74" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B74" s="36" t="s">
+        <v>286</v>
+      </c>
+      <c r="C74" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="D74" s="26" t="s">
+        <v>256</v>
+      </c>
+      <c r="E74" s="24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" s="27" customFormat="1">
+      <c r="A75" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B75" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="C75" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="D75" s="26" t="s">
         <v>266</v>
       </c>
-      <c r="E57" s="24" t="s">
-        <v>261</v>
-      </c>
-      <c r="F57" s="27" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" s="27" customFormat="1" ht="42">
-      <c r="A58" s="24" t="s">
-        <v>299</v>
-      </c>
-      <c r="B58" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="C58" s="24" t="s">
+      <c r="E75" s="24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" s="27" customFormat="1" ht="28">
+      <c r="A76" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B76" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="C76" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="D58" s="26" t="s">
-        <v>262</v>
-      </c>
-      <c r="E58" s="24" t="s">
-        <v>261</v>
-      </c>
-      <c r="F58" s="27" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" s="27" customFormat="1" ht="28">
-      <c r="A59" s="24" t="s">
-        <v>299</v>
-      </c>
-      <c r="B59" s="25" t="s">
-        <v>110</v>
-      </c>
-      <c r="C59" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="D59" s="26" t="s">
-        <v>263</v>
-      </c>
-      <c r="E59" s="24" t="s">
-        <v>261</v>
-      </c>
-      <c r="F59" s="27" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" s="27" customFormat="1" ht="28">
-      <c r="A60" s="24" t="s">
-        <v>299</v>
-      </c>
-      <c r="B60" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="C60" s="24" t="s">
-        <v>154</v>
-      </c>
-      <c r="D60" s="26" t="s">
+      <c r="D76" s="26" t="s">
+        <v>267</v>
+      </c>
+      <c r="E76" s="24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" s="27" customFormat="1">
+      <c r="A77" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B77" s="42" t="s">
+        <v>187</v>
+      </c>
+      <c r="C77" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="D77" s="26" t="s">
+        <v>276</v>
+      </c>
+      <c r="E77" s="24" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" s="27" customFormat="1" ht="28">
+      <c r="A78" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B78" s="41" t="s">
+        <v>288</v>
+      </c>
+      <c r="C78" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="D78" s="26" t="s">
+        <v>275</v>
+      </c>
+      <c r="E78" s="24" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" s="27" customFormat="1">
+      <c r="A79" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B79" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="C79" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="D79" s="26"/>
+      <c r="E79" s="24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" s="27" customFormat="1" ht="28">
+      <c r="A80" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B80" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="C80" s="24" t="s">
+        <v>183</v>
+      </c>
+      <c r="D80" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="E80" s="24" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" s="27" customFormat="1" ht="42">
+      <c r="A81" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B81" s="42" t="s">
+        <v>306</v>
+      </c>
+      <c r="C81" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="D81" s="26" t="s">
         <v>264</v>
       </c>
-      <c r="E60" s="24" t="s">
-        <v>261</v>
-      </c>
-      <c r="F60" s="27" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" s="27" customFormat="1" ht="28">
-      <c r="A61" s="24" t="s">
-        <v>299</v>
-      </c>
-      <c r="B61" s="25" t="s">
-        <v>156</v>
-      </c>
-      <c r="C61" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="D61" s="26" t="s">
-        <v>265</v>
-      </c>
-      <c r="E61" s="24" t="s">
-        <v>261</v>
-      </c>
-      <c r="F61" s="27" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" s="27" customFormat="1">
-      <c r="A62" s="24" t="s">
-        <v>299</v>
-      </c>
-      <c r="B62" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="C62" s="24" t="s">
-        <v>159</v>
-      </c>
-      <c r="D62" s="26" t="s">
-        <v>268</v>
-      </c>
-      <c r="E62" s="24" t="s">
-        <v>261</v>
-      </c>
-      <c r="F62" s="27" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" s="27" customFormat="1">
-      <c r="A63" s="24" t="s">
-        <v>299</v>
-      </c>
-      <c r="B63" s="25" t="s">
-        <v>115</v>
-      </c>
-      <c r="C63" s="24" t="s">
+      <c r="E81" s="24" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" s="27" customFormat="1">
+      <c r="A82" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B82" s="41" t="s">
+        <v>289</v>
+      </c>
+      <c r="C82" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="D82" s="26" t="s">
+        <v>257</v>
+      </c>
+      <c r="E82" s="24" t="s">
         <v>47</v>
-      </c>
-      <c r="D63" s="26" t="s">
-        <v>269</v>
-      </c>
-      <c r="E63" s="24" t="s">
-        <v>261</v>
-      </c>
-      <c r="F63" s="27" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" s="27" customFormat="1" ht="42">
-      <c r="A64" s="24" t="s">
-        <v>299</v>
-      </c>
-      <c r="B64" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="C64" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="D64" s="26" t="s">
-        <v>267</v>
-      </c>
-      <c r="E64" s="24" t="s">
-        <v>261</v>
-      </c>
-      <c r="F64" s="27" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" s="27" customFormat="1" ht="28">
-      <c r="A65" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B65" s="25" t="s">
-        <v>190</v>
-      </c>
-      <c r="C65" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="D65" s="26" t="s">
-        <v>276</v>
-      </c>
-      <c r="E65" s="24" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" s="27" customFormat="1">
-      <c r="A66" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B66" s="25" t="s">
-        <v>153</v>
-      </c>
-      <c r="C66" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="D66" s="26" t="s">
-        <v>285</v>
-      </c>
-      <c r="E66" s="24" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" s="27" customFormat="1">
-      <c r="A67" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B67" s="25" t="s">
-        <v>249</v>
-      </c>
-      <c r="C67" s="24" t="s">
-        <v>157</v>
-      </c>
-      <c r="D67" s="26"/>
-      <c r="E67" s="24" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" s="27" customFormat="1" ht="28">
-      <c r="A68" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B68" s="25" t="s">
-        <v>191</v>
-      </c>
-      <c r="C68" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="D68" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="E68" s="24" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" s="27" customFormat="1" ht="28">
-      <c r="A69" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B69" s="25" t="s">
-        <v>117</v>
-      </c>
-      <c r="C69" s="24" t="s">
-        <v>194</v>
-      </c>
-      <c r="D69" s="26" t="s">
-        <v>297</v>
-      </c>
-      <c r="E69" s="24" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" s="27" customFormat="1" ht="28">
-      <c r="A70" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B70" s="25" t="s">
-        <v>193</v>
-      </c>
-      <c r="C70" s="24" t="s">
-        <v>192</v>
-      </c>
-      <c r="D70" s="26" t="s">
-        <v>277</v>
-      </c>
-      <c r="E70" s="24" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" s="27" customFormat="1" ht="28">
-      <c r="A71" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B71" s="25" t="s">
-        <v>248</v>
-      </c>
-      <c r="C71" s="24" t="s">
-        <v>168</v>
-      </c>
-      <c r="D71" s="26" t="s">
-        <v>278</v>
-      </c>
-      <c r="E71" s="24" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" s="27" customFormat="1" ht="28">
-      <c r="A72" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B72" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="C72" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="D72" s="26" t="s">
-        <v>286</v>
-      </c>
-      <c r="E72" s="24" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" s="27" customFormat="1">
-      <c r="A73" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B73" s="25" t="s">
-        <v>250</v>
-      </c>
-      <c r="C73" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="D73" s="26" t="s">
-        <v>279</v>
-      </c>
-      <c r="E73" s="24" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" s="27" customFormat="1" ht="28">
-      <c r="A74" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B74" s="25" t="s">
-        <v>165</v>
-      </c>
-      <c r="C74" s="24" t="s">
-        <v>259</v>
-      </c>
-      <c r="D74" s="26" t="s">
-        <v>280</v>
-      </c>
-      <c r="E74" s="24" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" s="27" customFormat="1" ht="28">
-      <c r="A75" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B75" s="25" t="s">
-        <v>251</v>
-      </c>
-      <c r="C75" s="24" t="s">
-        <v>166</v>
-      </c>
-      <c r="D75" s="26" t="s">
-        <v>281</v>
-      </c>
-      <c r="E75" s="24" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" s="27" customFormat="1" ht="28">
-      <c r="A76" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B76" s="25" t="s">
-        <v>109</v>
-      </c>
-      <c r="C76" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="D76" s="26" t="s">
-        <v>294</v>
-      </c>
-      <c r="E76" s="24" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" s="27" customFormat="1" ht="42">
-      <c r="A77" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B77" s="25"/>
-      <c r="C77" s="28" t="s">
-        <v>158</v>
-      </c>
-      <c r="D77" s="26" t="s">
-        <v>282</v>
-      </c>
-      <c r="E77" s="24" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" s="27" customFormat="1">
-      <c r="A78" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B78" s="25" t="s">
-        <v>195</v>
-      </c>
-      <c r="C78" s="28" t="s">
-        <v>169</v>
-      </c>
-      <c r="D78" s="26" t="s">
-        <v>287</v>
-      </c>
-      <c r="E78" s="24" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" s="27" customFormat="1">
-      <c r="A79" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B79" s="25" t="s">
-        <v>196</v>
-      </c>
-      <c r="C79" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="D79" s="26" t="s">
-        <v>295</v>
-      </c>
-      <c r="E79" s="24" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" s="27" customFormat="1">
-      <c r="A80" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B80" s="25" t="s">
-        <v>252</v>
-      </c>
-      <c r="C80" s="24" t="s">
-        <v>160</v>
-      </c>
-      <c r="D80" s="26" t="s">
-        <v>288</v>
-      </c>
-      <c r="E80" s="24" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" s="27" customFormat="1">
-      <c r="A81" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B81" s="25" t="s">
-        <v>253</v>
-      </c>
-      <c r="C81" s="24" t="s">
-        <v>247</v>
-      </c>
-      <c r="D81" s="26" t="s">
-        <v>289</v>
-      </c>
-      <c r="E81" s="24" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" s="27" customFormat="1" ht="28">
-      <c r="A82" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B82" s="25" t="s">
-        <v>254</v>
-      </c>
-      <c r="C82" s="24" t="s">
-        <v>161</v>
-      </c>
-      <c r="D82" s="26" t="s">
-        <v>290</v>
-      </c>
-      <c r="E82" s="24" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="83" spans="1:5" s="27" customFormat="1">
       <c r="A83" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B83" s="25" t="s">
-        <v>255</v>
+        <v>188</v>
+      </c>
+      <c r="B83" s="42" t="s">
+        <v>241</v>
       </c>
       <c r="C83" s="24" t="s">
-        <v>162</v>
-      </c>
-      <c r="D83" s="26"/>
+        <v>156</v>
+      </c>
+      <c r="D83" s="26" t="s">
+        <v>254</v>
+      </c>
       <c r="E83" s="24" t="s">
-        <v>159</v>
+        <v>62</v>
       </c>
     </row>
     <row r="84" spans="1:5" s="27" customFormat="1" ht="28">
       <c r="A84" s="24" t="s">
-        <v>50</v>
+        <v>188</v>
       </c>
       <c r="B84" s="25" t="s">
-        <v>142</v>
-      </c>
-      <c r="C84" s="28" t="s">
-        <v>291</v>
+        <v>236</v>
+      </c>
+      <c r="C84" s="24" t="s">
+        <v>159</v>
       </c>
       <c r="D84" s="26" t="s">
-        <v>292</v>
+        <v>260</v>
       </c>
       <c r="E84" s="24" t="s">
-        <v>47</v>
+        <v>158</v>
       </c>
     </row>
     <row r="85" spans="1:5" s="27" customFormat="1">
       <c r="A85" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B85" s="25" t="s">
-        <v>105</v>
+        <v>188</v>
+      </c>
+      <c r="B85" s="36" t="s">
+        <v>293</v>
       </c>
       <c r="C85" s="24" t="s">
-        <v>86</v>
+        <v>155</v>
       </c>
       <c r="D85" s="26" t="s">
-        <v>274</v>
+        <v>255</v>
       </c>
       <c r="E85" s="24" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
     </row>
     <row r="86" spans="1:5" s="27" customFormat="1">
       <c r="A86" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B86" s="25" t="s">
-        <v>67</v>
+        <v>188</v>
+      </c>
+      <c r="B86" s="36" t="s">
+        <v>294</v>
       </c>
       <c r="C86" s="24" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D86" s="26" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="E86" s="24" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" s="27" customFormat="1" ht="28">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" s="27" customFormat="1">
       <c r="A87" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B87" s="36" t="s">
-        <v>106</v>
+        <v>188</v>
+      </c>
+      <c r="B87" s="42" t="s">
+        <v>239</v>
       </c>
       <c r="C87" s="24" t="s">
-        <v>66</v>
+        <v>235</v>
       </c>
       <c r="D87" s="26" t="s">
-        <v>293</v>
+        <v>270</v>
       </c>
       <c r="E87" s="24" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" s="27" customFormat="1" ht="28">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" s="27" customFormat="1">
       <c r="A88" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B88" s="25" t="s">
-        <v>256</v>
-      </c>
-      <c r="C88" s="24" t="s">
-        <v>70</v>
+        <v>188</v>
+      </c>
+      <c r="B88" s="42" t="s">
+        <v>186</v>
+      </c>
+      <c r="C88" s="28" t="s">
+        <v>160</v>
       </c>
       <c r="D88" s="26" t="s">
+        <v>268</v>
+      </c>
+      <c r="E88" s="24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" s="27" customFormat="1" ht="28">
+      <c r="A89" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B89" s="25" t="s">
+        <v>238</v>
+      </c>
+      <c r="C89" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="D89" s="26" t="s">
+        <v>263</v>
+      </c>
+      <c r="E89" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" s="27" customFormat="1" ht="28">
+      <c r="A90" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B90" s="41" t="s">
+        <v>281</v>
+      </c>
+      <c r="C90" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="D90" s="26" t="s">
+        <v>271</v>
+      </c>
+      <c r="E90" s="24" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" s="27" customFormat="1">
+      <c r="A91" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B91" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="C91" s="29" t="s">
+        <v>359</v>
+      </c>
+      <c r="D91" s="30"/>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B92" s="22" t="s">
+        <v>292</v>
+      </c>
+      <c r="C92" s="22" t="s">
+        <v>345</v>
+      </c>
+      <c r="D92" s="22" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B93" s="22" t="s">
+        <v>295</v>
+      </c>
+      <c r="C93" s="22" t="s">
+        <v>357</v>
+      </c>
+      <c r="D93" s="22" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B94" s="22" t="s">
         <v>296</v>
       </c>
-      <c r="E88" s="24" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" s="27" customFormat="1">
-      <c r="A89" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B89" s="25" t="s">
-        <v>258</v>
-      </c>
-      <c r="C89" s="24" t="s">
-        <v>164</v>
-      </c>
-      <c r="D89" s="26" t="s">
-        <v>272</v>
-      </c>
-      <c r="E89" s="24" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" s="27" customFormat="1">
-      <c r="A90" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B90" s="25" t="s">
-        <v>257</v>
-      </c>
-      <c r="C90" s="24" t="s">
-        <v>163</v>
-      </c>
-      <c r="D90" s="26" t="s">
-        <v>273</v>
-      </c>
-      <c r="E90" s="24" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" s="27" customFormat="1">
-      <c r="C91" s="29"/>
-      <c r="D91" s="30"/>
+      <c r="C94" s="22" t="s">
+        <v>316</v>
+      </c>
+      <c r="D94" s="22" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B95" s="22" t="s">
+        <v>297</v>
+      </c>
+      <c r="C95" s="22" t="s">
+        <v>317</v>
+      </c>
+      <c r="D95" s="22" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B96" s="22" t="s">
+        <v>298</v>
+      </c>
+      <c r="C96" s="22" t="s">
+        <v>318</v>
+      </c>
+      <c r="D96" s="22" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B97" s="22" t="s">
+        <v>299</v>
+      </c>
+      <c r="C97" s="22" t="s">
+        <v>319</v>
+      </c>
+      <c r="D97" s="22" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B98" s="22" t="s">
+        <v>300</v>
+      </c>
+      <c r="C98" s="22" t="s">
+        <v>320</v>
+      </c>
+      <c r="D98" s="22" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="28">
+      <c r="A99" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="C99" s="36" t="s">
+        <v>344</v>
+      </c>
+      <c r="D99" s="22" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="28">
+      <c r="A100" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="C100" s="36" t="s">
+        <v>346</v>
+      </c>
+      <c r="D100" s="22" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="28">
+      <c r="A101" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="C101" s="36" t="s">
+        <v>347</v>
+      </c>
+      <c r="D101" s="26" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="C102" s="36" t="s">
+        <v>342</v>
+      </c>
+      <c r="D102" s="22" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="28">
+      <c r="A103" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="C103" s="36" t="s">
+        <v>332</v>
+      </c>
+      <c r="D103" s="26" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="C104" s="36" t="s">
+        <v>327</v>
+      </c>
+      <c r="D104" s="22" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="28">
+      <c r="A105" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="C105" s="36" t="s">
+        <v>330</v>
+      </c>
+      <c r="D105" s="22" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
+      <c r="A106" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="C106" s="36" t="s">
+        <v>331</v>
+      </c>
+      <c r="D106" s="22" t="s">
+        <v>368</v>
+      </c>
+      <c r="E106" s="21" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
+      <c r="A107" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="C107" s="36" t="s">
+        <v>323</v>
+      </c>
+      <c r="D107" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="E107" s="21" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="28">
+      <c r="A108" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B108" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C108" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D108" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="E108" s="21" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
+      <c r="A109" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="C109" s="36" t="s">
+        <v>348</v>
+      </c>
+      <c r="D109" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="E109" s="21" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="28">
+      <c r="A110" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B110" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="C110" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="D110" s="23" t="s">
+        <v>219</v>
+      </c>
+      <c r="E110" s="21" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="42">
+      <c r="A111" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B111" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="C111" s="36" t="s">
+        <v>333</v>
+      </c>
+      <c r="D111" s="52" t="s">
+        <v>372</v>
+      </c>
+      <c r="E111" s="21" t="s">
+        <v>361</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="C165:C173">
-    <sortCondition ref="C165"/>
+  <sortState ref="B92:B101">
+    <sortCondition ref="B92"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="F15" r:id="rId1" display="http://www.ktponline.org.uk/technology-strategy-board"/>
-    <hyperlink ref="F23" r:id="rId2"/>
-    <hyperlink ref="F19" r:id="rId3"/>
-    <hyperlink ref="F13" r:id="rId4"/>
-    <hyperlink ref="F17" r:id="rId5"/>
-    <hyperlink ref="F26" r:id="rId6"/>
+    <hyperlink ref="F16" r:id="rId1" display="http://www.ktponline.org.uk/technology-strategy-board"/>
+    <hyperlink ref="F24" r:id="rId2"/>
+    <hyperlink ref="F20" r:id="rId3"/>
+    <hyperlink ref="F14" r:id="rId4"/>
+    <hyperlink ref="F18" r:id="rId5"/>
+    <hyperlink ref="F27" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -3462,4 +4069,883 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K49"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K33" sqref="K33:K34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="52.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" style="49"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="B1" t="s">
+        <v>321</v>
+      </c>
+      <c r="D1" s="49" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="46">
+        <v>1</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="48" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="46">
+        <v>2</v>
+      </c>
+      <c r="B3" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="43"/>
+      <c r="D3" s="48" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="46">
+        <v>3</v>
+      </c>
+      <c r="B4" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="43"/>
+      <c r="D4" s="48" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="46">
+        <v>4</v>
+      </c>
+      <c r="B5" s="47" t="s">
+        <v>272</v>
+      </c>
+      <c r="C5" s="43"/>
+      <c r="D5" s="48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="46">
+        <v>5</v>
+      </c>
+      <c r="B6" s="47" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="43"/>
+      <c r="D6" s="48" t="s">
+        <v>73</v>
+      </c>
+      <c r="K6" s="48" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="46"/>
+      <c r="B7" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="43"/>
+      <c r="K7" s="48" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="46">
+        <v>6</v>
+      </c>
+      <c r="B8" s="47" t="s">
+        <v>242</v>
+      </c>
+      <c r="C8" s="43"/>
+      <c r="D8" s="48" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="46"/>
+      <c r="B9" s="47" t="s">
+        <v>185</v>
+      </c>
+      <c r="C9" s="43"/>
+      <c r="D9" s="48" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="46">
+        <v>7</v>
+      </c>
+      <c r="B10" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="43"/>
+      <c r="D10" s="48" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="46"/>
+      <c r="B11" s="47" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="43"/>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="46"/>
+      <c r="B12" s="47" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="43"/>
+      <c r="D12" s="48" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="46"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="48" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="46"/>
+      <c r="B14" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" s="43"/>
+      <c r="D14" s="48"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="46"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="48" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="46"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="48" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="46"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="48" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="46"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="48" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="46"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="K19" s="48" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="46">
+        <v>8</v>
+      </c>
+      <c r="B20" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="43"/>
+      <c r="D20" s="48" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="46"/>
+      <c r="B21" s="47" t="s">
+        <v>149</v>
+      </c>
+      <c r="C21" s="43"/>
+      <c r="D21" s="48"/>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="46"/>
+      <c r="B22" s="47" t="s">
+        <v>183</v>
+      </c>
+      <c r="C22" s="43"/>
+      <c r="D22" s="48"/>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" s="46">
+        <v>9</v>
+      </c>
+      <c r="B23" s="47" t="s">
+        <v>147</v>
+      </c>
+      <c r="C23" s="44"/>
+      <c r="D23" s="48" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="46"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="48" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" s="46"/>
+      <c r="B25" s="47" t="s">
+        <v>156</v>
+      </c>
+      <c r="C25" s="45"/>
+      <c r="D25" s="48" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" s="46"/>
+      <c r="B26" s="47" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" s="46"/>
+      <c r="B27" s="47" t="s">
+        <v>150</v>
+      </c>
+      <c r="K27" s="48" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" s="46"/>
+      <c r="D28" s="48" t="s">
+        <v>338</v>
+      </c>
+      <c r="K28" s="48"/>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" s="46">
+        <v>10</v>
+      </c>
+      <c r="B29" s="47" t="s">
+        <v>316</v>
+      </c>
+      <c r="D29" s="48" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" s="46">
+        <v>11</v>
+      </c>
+      <c r="B30" s="47" t="s">
+        <v>317</v>
+      </c>
+      <c r="D30" s="48" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" s="46">
+        <v>12</v>
+      </c>
+      <c r="B31" s="47" t="s">
+        <v>318</v>
+      </c>
+      <c r="D31" s="48" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" s="46"/>
+      <c r="D32" s="48" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" s="46">
+        <v>13</v>
+      </c>
+      <c r="B33" s="47" t="s">
+        <v>137</v>
+      </c>
+      <c r="K33" s="48" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" s="46"/>
+      <c r="K34" s="48" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" s="46">
+        <v>14</v>
+      </c>
+      <c r="B35" s="47" t="s">
+        <v>315</v>
+      </c>
+      <c r="D35" s="48" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36" s="46"/>
+      <c r="D36" s="48" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" s="46">
+        <v>15</v>
+      </c>
+      <c r="B37" s="47" t="s">
+        <v>155</v>
+      </c>
+      <c r="D37" s="48" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38" s="46">
+        <v>16</v>
+      </c>
+      <c r="B38" s="47" t="s">
+        <v>152</v>
+      </c>
+      <c r="D38" s="48" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="D39" s="48" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40" s="50">
+        <v>17</v>
+      </c>
+      <c r="B40" s="47" t="s">
+        <v>319</v>
+      </c>
+      <c r="D40" s="48" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="A41" s="50">
+        <v>18</v>
+      </c>
+      <c r="B41" s="47" t="s">
+        <v>320</v>
+      </c>
+      <c r="D41" s="48" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="B42" s="47" t="s">
+        <v>235</v>
+      </c>
+      <c r="D42" s="48"/>
+      <c r="K42" s="48" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="B43" s="47" t="s">
+        <v>160</v>
+      </c>
+      <c r="D43" s="48" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="A44">
+        <v>19</v>
+      </c>
+      <c r="B44" s="47" t="s">
+        <v>157</v>
+      </c>
+      <c r="D44" s="48" t="s">
+        <v>157</v>
+      </c>
+      <c r="K44" s="48" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="D45" s="48" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46">
+        <v>20</v>
+      </c>
+      <c r="B46" s="47" t="s">
+        <v>153</v>
+      </c>
+      <c r="D46" s="48" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="D47" s="48" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="D48" s="48" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2">
+      <c r="B49" s="47" t="s">
+        <v>154</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="C4:C22">
+    <sortCondition ref="C3"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:E47"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="58.5" style="49" customWidth="1"/>
+    <col min="4" max="4" width="52.6640625" customWidth="1"/>
+    <col min="5" max="5" width="40.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5">
+      <c r="B1" s="51" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5">
+      <c r="B2" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5">
+      <c r="B3" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5">
+      <c r="B4" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5">
+      <c r="B5" s="36" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" s="36" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5">
+      <c r="B8" s="36" t="s">
+        <v>324</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5">
+      <c r="B9" s="36" t="s">
+        <v>325</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5">
+      <c r="B10" s="36" t="s">
+        <v>326</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="B11" s="36" t="s">
+        <v>327</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5">
+      <c r="B12" s="36" t="s">
+        <v>328</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5">
+      <c r="B13" s="36" t="s">
+        <v>329</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5">
+      <c r="B14" s="36" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5">
+      <c r="B15" s="36" t="s">
+        <v>331</v>
+      </c>
+      <c r="D15" s="24"/>
+    </row>
+    <row r="16" spans="2:5">
+      <c r="B16" s="36" t="s">
+        <v>332</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="B17" s="36" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5">
+      <c r="B18" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="B19" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="24" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5">
+      <c r="B20" s="36" t="s">
+        <v>334</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="E20" s="24" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5">
+      <c r="B21" s="36" t="s">
+        <v>335</v>
+      </c>
+      <c r="E21" s="28" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5">
+      <c r="B22" s="36" t="s">
+        <v>336</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5">
+      <c r="B23" s="36" t="s">
+        <v>337</v>
+      </c>
+      <c r="D23" s="24" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5">
+      <c r="B24" s="36" t="s">
+        <v>338</v>
+      </c>
+      <c r="D24" s="22" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5">
+      <c r="B25" s="36" t="s">
+        <v>339</v>
+      </c>
+      <c r="D25" s="22" t="s">
+        <v>316</v>
+      </c>
+      <c r="E25" s="24" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5">
+      <c r="B26" s="36" t="s">
+        <v>340</v>
+      </c>
+      <c r="D26" s="22" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5">
+      <c r="B27" s="36" t="s">
+        <v>341</v>
+      </c>
+      <c r="D27" s="22" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5">
+      <c r="B28" s="36" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5">
+      <c r="B29" s="36" t="s">
+        <v>343</v>
+      </c>
+      <c r="D29" s="22" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5">
+      <c r="B30" s="36" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5">
+      <c r="B31" s="36" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5">
+      <c r="B32" s="36" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5">
+      <c r="B33" s="36" t="s">
+        <v>155</v>
+      </c>
+      <c r="D33" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="E33" s="24" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5">
+      <c r="B34" s="36" t="s">
+        <v>152</v>
+      </c>
+      <c r="D34" s="24" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5">
+      <c r="B35" s="36" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5">
+      <c r="B36" s="36" t="s">
+        <v>319</v>
+      </c>
+      <c r="D36" s="22" t="s">
+        <v>319</v>
+      </c>
+      <c r="E36" s="24" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5">
+      <c r="B37" s="36" t="s">
+        <v>320</v>
+      </c>
+      <c r="D37" s="22" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5">
+      <c r="B38" s="36" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5">
+      <c r="B39" s="36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5">
+      <c r="B40" s="36" t="s">
+        <v>349</v>
+      </c>
+      <c r="D40" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="E40" s="28" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5">
+      <c r="B41" s="36" t="s">
+        <v>157</v>
+      </c>
+      <c r="D41" s="24" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5">
+      <c r="B42" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="D42" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="E42" s="24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5">
+      <c r="B43" s="36" t="s">
+        <v>350</v>
+      </c>
+      <c r="D43" s="24" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5">
+      <c r="B44" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="D44" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5">
+      <c r="B45" s="36" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5">
+      <c r="B46" s="36" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5">
+      <c r="E47" s="24" t="s">
+        <v>154</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="D2:D44">
+    <sortCondition ref="D2"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>